<commit_message>
(C)    r2 of lifting plan
</commit_message>
<xml_diff>
--- a/Suppl/lifting plan.xlsx
+++ b/Suppl/lifting plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Me\Fitness\Suppl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>Src</t>
   </si>
@@ -276,7 +276,46 @@
     <t>Soft Target (2 months)</t>
   </si>
   <si>
-    <t>(11/15/16)</t>
+    <t>(11/15/16) r2</t>
+  </si>
+  <si>
+    <t>Dumbbell Bench Flys</t>
+  </si>
+  <si>
+    <t>Reverse Flys</t>
+  </si>
+  <si>
+    <t>Lunge</t>
+  </si>
+  <si>
+    <t>Chinup</t>
+  </si>
+  <si>
+    <t>Deadlift</t>
+  </si>
+  <si>
+    <t>Shoulder Press</t>
+  </si>
+  <si>
+    <t>Calf Raise</t>
+  </si>
+  <si>
+    <t>Cable Baseball Swing</t>
+  </si>
+  <si>
+    <t>Hip Adduction</t>
+  </si>
+  <si>
+    <t>Hip Abduction</t>
+  </si>
+  <si>
+    <t>Chest (9)</t>
+  </si>
+  <si>
+    <t>Lower (7)</t>
+  </si>
+  <si>
+    <t>Arms (8)</t>
   </si>
 </sst>
 </file>
@@ -335,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -348,6 +387,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,12 +708,12 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="G30" sqref="E1:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -702,7 +744,7 @@
       <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="11">
         <v>42689</v>
       </c>
       <c r="C3" s="1"/>
@@ -730,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
@@ -738,7 +780,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -793,79 +835,89 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="3"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>21</v>
+      <c r="B22" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -882,7 +934,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -931,12 +983,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
(C)    update to lower, lunges added and others
</commit_message>
<xml_diff>
--- a/Suppl/lifting plan.xlsx
+++ b/Suppl/lifting plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="127">
   <si>
     <t>Src</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Calf Raise</t>
   </si>
   <si>
-    <t>Cable Baseball Swing</t>
-  </si>
-  <si>
     <t>Hip Adduction</t>
   </si>
   <si>
@@ -372,15 +369,9 @@
     <t>(Machine Revese Fky)</t>
   </si>
   <si>
-    <t>(11/19/16) r4</t>
-  </si>
-  <si>
     <t>(Selectorized Leg Press)</t>
   </si>
   <si>
-    <t>(Selectorized Leg Curl)</t>
-  </si>
-  <si>
     <t>(Abdominal Crunches)</t>
   </si>
   <si>
@@ -396,17 +387,32 @@
     <t>(Standing, Single Leg Dumbbell Calf Raise)</t>
   </si>
   <si>
-    <t>(Cable Baseball Swing)</t>
-  </si>
-  <si>
-    <t>(Stairs Dumbbell Step-Up)</t>
+    <t>Single Leg Extensions</t>
+  </si>
+  <si>
+    <t>Single Leg Curls</t>
+  </si>
+  <si>
+    <t>Lunges</t>
+  </si>
+  <si>
+    <t>(11/23/16) r5</t>
+  </si>
+  <si>
+    <t>(Bodyweight Lunge)</t>
+  </si>
+  <si>
+    <t>(Selectorized Individual Leg Curl)</t>
+  </si>
+  <si>
+    <t>(Selectorized Individual Leg Extension)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +430,14 @@
     </font>
     <font>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -465,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -484,6 +498,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,10 +854,10 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
         <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -867,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
@@ -879,7 +894,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -889,7 +904,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -899,7 +914,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,7 +924,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,7 +934,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,7 +944,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -939,7 +954,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,7 +964,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,7 +974,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,153 +986,159 @@
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
-        <v>69</v>
+      <c r="B19" t="s">
+        <v>122</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="3"/>
       <c r="D21" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="3"/>
       <c r="D26" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1127,7 +1148,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1137,7 +1158,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1147,7 +1168,7 @@
       </c>
       <c r="C35" s="3"/>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1157,17 +1178,17 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1182,7 +1203,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="10" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(C)    updated/corrected a few lifts, cleaned up doc
</commit_message>
<xml_diff>
--- a/Suppl/lifting plan.xlsx
+++ b/Suppl/lifting plan.xlsx
@@ -333,18 +333,9 @@
     <t>(Barbell Bench Press Flat)</t>
   </si>
   <si>
-    <t>(Cable Fly Seated)</t>
-  </si>
-  <si>
     <t>(Selectorized Row)</t>
   </si>
   <si>
-    <t>(Barbell Raise)</t>
-  </si>
-  <si>
-    <t>(Dumbbell Biceps Curl (Underhand Grip)</t>
-  </si>
-  <si>
     <t>(Dumbbell Wrist Curl)</t>
   </si>
   <si>
@@ -366,9 +357,6 @@
     <t>(Selectorized Hyperextension)</t>
   </si>
   <si>
-    <t>(Machine Revese Fky)</t>
-  </si>
-  <si>
     <t>(Selectorized Leg Press)</t>
   </si>
   <si>
@@ -396,9 +384,6 @@
     <t>Lunges</t>
   </si>
   <si>
-    <t>(11/23/16) r5</t>
-  </si>
-  <si>
     <t>(Bodyweight Lunge)</t>
   </si>
   <si>
@@ -406,6 +391,21 @@
   </si>
   <si>
     <t>(Selectorized Individual Leg Extension)</t>
+  </si>
+  <si>
+    <t>(11/24/16) r6</t>
+  </si>
+  <si>
+    <t>(Selectorized Fly)</t>
+  </si>
+  <si>
+    <t>(Barbbell Raise)</t>
+  </si>
+  <si>
+    <t>(Machine Revese Fly)</t>
+  </si>
+  <si>
+    <t>(Dumbbell Biceps Curl (Underhand Grip))</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -991,98 +991,104 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>114</v>
+        <v>58</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>124</v>
+      <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
+      <c r="B20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>115</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" t="s">
-        <v>88</v>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="13" t="s">
-        <v>116</v>
+      <c r="D22" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" t="s">
-        <v>89</v>
+      <c r="B23" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="13" t="s">
-        <v>117</v>
+      <c r="D23" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" t="s">
-        <v>120</v>
-      </c>
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="3"/>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>118</v>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" t="s">
+        <v>107</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="14"/>
+      <c r="B26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
@@ -1096,100 +1102,94 @@
         <v>31</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" t="s">
-        <v>105</v>
+        <v>68</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" t="s">
-        <v>109</v>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="3"/>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" t="s">
-        <v>107</v>
+        <v>71</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="3" t="s">
-        <v>70</v>
+      <c r="B33" t="s">
+        <v>88</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" t="s">
-        <v>108</v>
+      <c r="D33" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="3" t="s">
-        <v>76</v>
+      <c r="B34" t="s">
+        <v>89</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" t="s">
-        <v>112</v>
+      <c r="D34" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="3"/>
+      <c r="B35" t="s">
+        <v>116</v>
+      </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" t="s">
-        <v>110</v>
+      <c r="B36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" t="s">
-        <v>111</v>
-      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="14"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(C)    lift change updates, to match equipment on hand
</commit_message>
<xml_diff>
--- a/Suppl/lifting plan.xlsx
+++ b/Suppl/lifting plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -324,15 +324,9 @@
     <t>(Cable Lat Pulldown)</t>
   </si>
   <si>
-    <t>(Barbell Shoulder Press)</t>
-  </si>
-  <si>
     <t>(Barbell Bench Press Incline)</t>
   </si>
   <si>
-    <t>(Barbell Bench Press Flat)</t>
-  </si>
-  <si>
     <t>(Selectorized Row)</t>
   </si>
   <si>
@@ -406,6 +400,12 @@
   </si>
   <si>
     <t>(Dumbbell Biceps Curl (Underhand Grip))</t>
+  </si>
+  <si>
+    <t>(Dumbbell Bench Press Flat)</t>
+  </si>
+  <si>
+    <t>(Machine Shoulder Press)</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,11 +890,11 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,7 +964,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1113,25 +1113,25 @@
         <v>68</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>71</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,16 +1160,16 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>66</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>87</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E37" s="14"/>
     </row>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(+)    added Hammer Curls
</commit_message>
<xml_diff>
--- a/Suppl/lifting plan.xlsx
+++ b/Suppl/lifting plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="129">
   <si>
     <t>Src</t>
   </si>
@@ -387,9 +387,6 @@
     <t>(Selectorized Individual Leg Extension)</t>
   </si>
   <si>
-    <t>(11/24/16) r6</t>
-  </si>
-  <si>
     <t>(Selectorized Fly)</t>
   </si>
   <si>
@@ -406,6 +403,15 @@
   </si>
   <si>
     <t>(Machine Shoulder Press)</t>
+  </si>
+  <si>
+    <t>Hammer Curls</t>
+  </si>
+  <si>
+    <t>(Hammer Curl, Standing)</t>
+  </si>
+  <si>
+    <t>(12/7/16) r7</t>
   </si>
 </sst>
 </file>
@@ -813,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +900,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -914,7 +920,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -954,7 +960,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,7 +970,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,7 +1009,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1058,152 +1064,161 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="3"/>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
       <c r="D24" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
+        <v>127</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" t="s">
-        <v>86</v>
+      <c r="B25" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>92</v>
+      <c r="B26" t="s">
+        <v>86</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="C27" s="3"/>
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
+        <v>116</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>109</v>
+      <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="D33" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" t="s">
-        <v>119</v>
+        <v>89</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>112</v>
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" t="s">
-        <v>87</v>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="14"/>
+        <v>112</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="14"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I45" s="10" t="s">
-        <v>120</v>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>